<commit_message>
completed all the modules
</commit_message>
<xml_diff>
--- a/QVC/QVC_Dev/data/TestData.xlsx
+++ b/QVC/QVC_Dev/data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thamarais\git\QVC_DEV\QVC\QVC_Dev\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540FCF3B-13CF-42A1-A52A-A3909C58C857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E107ED-636F-4FDB-9C77-E424B7DF2280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,22 +81,22 @@
     <t xml:space="preserve">27 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 10:00</t>
-  </si>
-  <si>
-    <t>523456INDNWC</t>
-  </si>
-  <si>
-    <t>523456</t>
-  </si>
-  <si>
     <t>Reschedule_date</t>
   </si>
   <si>
     <t>Reschedule_Time</t>
   </si>
   <si>
-    <t xml:space="preserve"> 12:45</t>
+    <t xml:space="preserve"> 10:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11.00</t>
+  </si>
+  <si>
+    <t>99121212</t>
+  </si>
+  <si>
+    <t>991212126INDNWC</t>
   </si>
 </sst>
 </file>
@@ -428,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,10 +479,10 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -493,10 +493,10 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>13</v>
@@ -517,13 +517,13 @@
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included RANDINT in scheduling page
</commit_message>
<xml_diff>
--- a/QVC/QVC_Dev/data/TestData.xlsx
+++ b/QVC/QVC_Dev/data/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thamarais\git\QVC_DEV\QVC\QVC_Dev\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012C4AFB-ABC5-4740-BB3F-8298BC582874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A5D593-3228-4C0E-9BE8-2BE0B21CF221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>passportNumber</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Reschedule_Time</t>
   </si>
   <si>
-    <t xml:space="preserve"> 11:15</t>
-  </si>
-  <si>
     <t>866363INDNWC</t>
   </si>
   <si>
@@ -97,12 +94,25 @@
   </si>
   <si>
     <t xml:space="preserve"> 12.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10:00</t>
+  </si>
+  <si>
+    <t>211NWCIND</t>
+  </si>
+  <si>
+    <t>12929</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,20 +438,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375"/>
+    <col min="4" max="4" customWidth="true" width="16.28515625"/>
+    <col min="5" max="5" customWidth="true" width="17.7109375"/>
+    <col min="6" max="6" customWidth="true" width="30.140625"/>
+    <col min="7" max="7" customWidth="true" width="24.7109375"/>
+    <col min="10" max="10" customWidth="true" width="25.0"/>
+    <col min="12" max="12" customWidth="true" width="17.7109375"/>
+    <col min="13" max="13" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -493,10 +503,10 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>13</v>
@@ -514,16 +524,16 @@
         <v>16</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>